<commit_message>
Created new lab item. Changed dictionary and made new diagram.
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <workbookPr codeName="ЦяКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRYSTAL\source\repos\modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA549C2B-06D5-4F9F-B222-02AEB8DA397A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67872250-CB2C-4E95-BC48-D5746FD65B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95FB1710-4561-4AB2-BA3B-49C7467EBABC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{95FB1710-4561-4AB2-BA3B-49C7467EBABC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="Тестовий" sheetId="1" r:id="rId1"/>
+    <sheet name="Лр2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Термін</t>
   </si>
@@ -150,6 +151,133 @@
   </si>
   <si>
     <t>пов'язує Group та Subject</t>
+  </si>
+  <si>
+    <t>об’єкт бібліотечного фонду, який містить інформацію (текстову чи іншу) та може бути виданий читачу</t>
+  </si>
+  <si>
+    <t>основна сутність</t>
+  </si>
+  <si>
+    <t>видання, примірник</t>
+  </si>
+  <si>
+    <t>книга “Мистецтво війни” віднесена до категорії історії</t>
+  </si>
+  <si>
+    <t>книга може мати кілька авторів та належати до однієї категорії.</t>
+  </si>
+  <si>
+    <t>фізична особа, що створила твір, представлений у вигляді книги</t>
+  </si>
+  <si>
+    <t>довідкова сутність</t>
+  </si>
+  <si>
+    <t>письменник</t>
+  </si>
+  <si>
+    <t>автор Іван Франко написав понад 100 творів</t>
+  </si>
+  <si>
+    <t>автор може бути співучасником написання кількох книг</t>
+  </si>
+  <si>
+    <t>книга (M:N)</t>
+  </si>
+  <si>
+    <t>користувач бібліотеки, який має право отримувати книги у тимчасове користування</t>
+  </si>
+  <si>
+    <t>користувач системи</t>
+  </si>
+  <si>
+    <t>абонент, користувач бібліотеки</t>
+  </si>
+  <si>
+    <t>читач Петренко Олег зарезервував три книги</t>
+  </si>
+  <si>
+    <t>читач може мати кілька замовлень одночасно</t>
+  </si>
+  <si>
+    <t>замовлення (1:N)</t>
+  </si>
+  <si>
+    <t>працівник бібліотеки, відповідальний за обслуговування читачів та управління фондами</t>
+  </si>
+  <si>
+    <t>працівник бібліотеки, оператор</t>
+  </si>
+  <si>
+    <t>бібліотекар видав книгу читачу та зареєстрував замовлення</t>
+  </si>
+  <si>
+    <t>один бібліотекар може обробляти багато замовлень</t>
+  </si>
+  <si>
+    <t>процес оформлення тимчасового користування книгою читачем</t>
+  </si>
+  <si>
+    <t>транзакційна сутність</t>
+  </si>
+  <si>
+    <t>позика, бронювання, оренда книги</t>
+  </si>
+  <si>
+    <t>замовлення №105 містить 2 книги й дату повернення 12.12.2025</t>
+  </si>
+  <si>
+    <t>зв’язує читача та книгу через бібліотекаря</t>
+  </si>
+  <si>
+    <t>читач (1:N)
+бібліотекар (1:N)
+книга (1:N)</t>
+  </si>
+  <si>
+    <t>тематична група книг у бібліотеці для класифікації та швидкого пошуку</t>
+  </si>
+  <si>
+    <t>жанр, рубрика, тематичний розділ</t>
+  </si>
+  <si>
+    <t>категорія “Наукова література” містить понад 300 книг</t>
+  </si>
+  <si>
+    <t>кожна книга належить тільки одній категорії</t>
+  </si>
+  <si>
+    <t>книга (1:N)</t>
+  </si>
+  <si>
+    <t>автор (M:N)
+категорія (1:N)
+замовлення (1:N)</t>
+  </si>
+  <si>
+    <t>Книга
+Book</t>
+  </si>
+  <si>
+    <t>Автор
+Author</t>
+  </si>
+  <si>
+    <t>Читач
+Reader</t>
+  </si>
+  <si>
+    <t>Бібліотекар
+Librarian</t>
+  </si>
+  <si>
+    <t>Замовлення
+Order</t>
+  </si>
+  <si>
+    <t>Категорія
+Category</t>
   </si>
 </sst>
 </file>
@@ -542,10 +670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933229EE-12C0-401E-9781-EDADAC85A6EB}">
+  <sheetPr codeName="Аркуш1"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,4 +823,186 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77760E3-73AC-4DE6-AC06-3F42B8E5948B}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
+    <col min="3" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="40.77734375" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>